<commit_message>
1. Add DocId tool implementation. 2. Display appropriate error message in the console. 3. Enable option to provide report path in the tool.
</commit_message>
<xml_diff>
--- a/Automation/LAAutomationTool/LAAutomationTool/bin/Debug/TestDataSheet.xlsx
+++ b/Automation/LAAutomationTool/LAAutomationTool/bin/Debug/TestDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Murali\Application\LAAutomationTool\LAAutomationTool\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7B3D55-0933-4ABA-AAF0-38CA89E6A09B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5666293-2AC5-491A-8CD3-E52CFB9EB704}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" xr2:uid="{0CDD1405-0FA4-469D-8768-C4FC7051CED5}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>